<commit_message>
added Point class and finished Game class
</commit_message>
<xml_diff>
--- a/Planung/klassendiagramm.xlsx
+++ b/Planung/klassendiagramm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NanoNode-Nexus\NanoNode-Nexus\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3E2A7D-491F-419E-B365-1A6A249ADB88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2030B9C4-B946-4AF1-9E6E-FAC9E51016AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{580508D2-892C-4584-8FAE-E54E01AF5A4F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>Entity : abstract</t>
   </si>
@@ -33,12 +33,6 @@
     <t>image: bmp</t>
   </si>
   <si>
-    <t>coords: pointer</t>
-  </si>
-  <si>
-    <t>dimensions: pointer</t>
-  </si>
-  <si>
     <t>setCoords(pointer): void</t>
   </si>
   <si>
@@ -60,12 +54,6 @@
     <t>getHP(): integer</t>
   </si>
   <si>
-    <t>getDimensions(): pointer</t>
-  </si>
-  <si>
-    <t>getCoords(): pointer</t>
-  </si>
-  <si>
     <t>getImage(): bmp</t>
   </si>
   <si>
@@ -159,9 +147,6 @@
     <t>getMapFromDB(levelName): grid</t>
   </si>
   <si>
-    <t>grid: Grid</t>
-  </si>
-  <si>
     <t>levelBuilder: LevelBuilder</t>
   </si>
   <si>
@@ -172,13 +157,79 @@
   </si>
   <si>
     <t>setRange(int): void</t>
+  </si>
+  <si>
+    <t>Tile</t>
+  </si>
+  <si>
+    <t>grid: Tile[][]</t>
+  </si>
+  <si>
+    <t>posX: int</t>
+  </si>
+  <si>
+    <t>posY: int</t>
+  </si>
+  <si>
+    <t>getPosX(): int</t>
+  </si>
+  <si>
+    <t>getPosY(): int</t>
+  </si>
+  <si>
+    <t>wallNorth: Wall</t>
+  </si>
+  <si>
+    <t>wallEast: Wall</t>
+  </si>
+  <si>
+    <t>wallSouth: Wall</t>
+  </si>
+  <si>
+    <t>wallWest: Wall</t>
+  </si>
+  <si>
+    <t>getWalls(): Walls[4]</t>
+  </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>x: int</t>
+  </si>
+  <si>
+    <t>y: int</t>
+  </si>
+  <si>
+    <t>x(): int</t>
+  </si>
+  <si>
+    <t>y(): int</t>
+  </si>
+  <si>
+    <t>setX(int): void</t>
+  </si>
+  <si>
+    <t>setY(int): void</t>
+  </si>
+  <si>
+    <t>position: Point</t>
+  </si>
+  <si>
+    <t>dimensions: Point</t>
+  </si>
+  <si>
+    <t>getPosition(): Point</t>
+  </si>
+  <si>
+    <t>getDimensions(): Point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,16 +237,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -320,11 +384,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -339,6 +429,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1154,66 +1248,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A199D6D-ABC7-45A7-B9CF-1C3816966CF7}">
-  <dimension ref="A2:Q33"/>
+  <dimension ref="A2:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="8"/>
       <c r="F3" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="8"/>
       <c r="J3" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="2"/>
       <c r="F4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="4"/>
       <c r="J4" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="4"/>
       <c r="F5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="4"/>
       <c r="J5" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="4"/>
@@ -1221,13 +1315,13 @@
       <c r="G6" s="10"/>
       <c r="H6" s="4"/>
       <c r="J6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="4"/>
@@ -1235,13 +1329,13 @@
       <c r="G7" s="10"/>
       <c r="H7" s="4"/>
       <c r="J7" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="6"/>
@@ -1250,10 +1344,12 @@
       <c r="H8" s="4"/>
       <c r="J8" s="3"/>
       <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O8" s="16"/>
+      <c r="Q8" s="14"/>
+    </row>
+    <row r="9" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="2"/>
@@ -1262,50 +1358,52 @@
       <c r="H9" s="4"/>
       <c r="J9" s="3"/>
       <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="O9" s="17"/>
+      <c r="Q9" s="15"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="4"/>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="4"/>
       <c r="F11" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="4"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="4"/>
       <c r="F12" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="4"/>
@@ -1313,9 +1411,9 @@
       <c r="G13" s="10"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="4"/>
@@ -1323,9 +1421,9 @@
       <c r="G14" s="10"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="6"/>
@@ -1333,60 +1431,70 @@
       <c r="G15" s="11"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="8"/>
       <c r="K18" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L18" s="12"/>
       <c r="M18" s="8"/>
       <c r="O18" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="P18" s="12"/>
       <c r="Q18" s="8"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" s="12"/>
+      <c r="U18" s="8"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B19" s="2"/>
       <c r="D19" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E19" s="8"/>
       <c r="G19" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="2"/>
       <c r="K19" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="4"/>
       <c r="O19" s="1" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T19" s="10"/>
+      <c r="U19" s="4"/>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B20" s="8"/>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E20" s="2"/>
       <c r="G20" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="4"/>
@@ -1394,20 +1502,25 @@
       <c r="L20" s="10"/>
       <c r="M20" s="4"/>
       <c r="O20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="4"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="T20" s="10"/>
+      <c r="U20" s="4"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="D21" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E21" s="4"/>
       <c r="G21" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H21" s="10"/>
       <c r="I21" s="4"/>
@@ -1417,50 +1530,65 @@
       <c r="O21" s="5"/>
       <c r="P21" s="11"/>
       <c r="Q21" s="6"/>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T21" s="10"/>
+      <c r="U21" s="4"/>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E22" s="6"/>
       <c r="G22" s="3"/>
       <c r="H22" s="10"/>
       <c r="I22" s="4"/>
       <c r="K22" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="2"/>
       <c r="O22" s="1"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T22" s="10"/>
+      <c r="U22" s="4"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E23" s="2"/>
       <c r="G23" s="5"/>
       <c r="H23" s="11"/>
       <c r="I23" s="6"/>
       <c r="K23" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="4"/>
       <c r="O23" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="4"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T23" s="10"/>
+      <c r="U23" s="4"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E24" s="4"/>
       <c r="G24" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="2"/>
@@ -1468,18 +1596,23 @@
       <c r="L24" s="10"/>
       <c r="M24" s="4"/>
       <c r="O24" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="4"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T24" s="10"/>
+      <c r="U24" s="4"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D25" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E25" s="4"/>
       <c r="G25" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="4"/>
@@ -1487,16 +1620,19 @@
       <c r="L25" s="10"/>
       <c r="M25" s="4"/>
       <c r="O25" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="4"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S25" s="3"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="4"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
       <c r="G26" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="4"/>
@@ -1506,12 +1642,15 @@
       <c r="O26" s="3"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="4"/>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S26" s="3"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="4"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="G27" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="4"/>
@@ -1521,38 +1660,111 @@
       <c r="O27" s="5"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="6"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S27" s="3"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="4"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G28" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T28" s="9"/>
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G29" s="3"/>
       <c r="H29" s="10"/>
       <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T29" s="10"/>
+      <c r="U29" s="4"/>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G30" s="3"/>
       <c r="H30" s="10"/>
       <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S30" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="T30" s="10"/>
+      <c r="U30" s="4"/>
+    </row>
+    <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G31" s="3"/>
       <c r="H31" s="10"/>
       <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P31" s="8"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="4"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G32" s="3"/>
       <c r="H32" s="10"/>
       <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P32" s="4"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="4"/>
+    </row>
+    <row r="33" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G33" s="5"/>
       <c r="H33" s="11"/>
       <c r="I33" s="6"/>
+      <c r="O33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P33" s="4"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="4"/>
+    </row>
+    <row r="34" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O34" s="5"/>
+      <c r="P34" s="6"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="4"/>
+    </row>
+    <row r="35" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P35" s="4"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="6"/>
+    </row>
+    <row r="36" spans="7:21" x14ac:dyDescent="0.25">
+      <c r="O36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="7:21" x14ac:dyDescent="0.25">
+      <c r="O37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P37" s="4"/>
+    </row>
+    <row r="38" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O38" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P38" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added maze generator and maze rendering, also placint entities in the middle according to grid
</commit_message>
<xml_diff>
--- a/Planung/klassendiagramm.xlsx
+++ b/Planung/klassendiagramm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NanoNode-Nexus\NanoNode-Nexus\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2030B9C4-B946-4AF1-9E6E-FAC9E51016AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFF80E2-9D68-44C1-92CF-A44AA0D64FED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{580508D2-892C-4584-8FAE-E54E01AF5A4F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Entity : abstract</t>
   </si>
@@ -159,37 +159,7 @@
     <t>setRange(int): void</t>
   </si>
   <si>
-    <t>Tile</t>
-  </si>
-  <si>
     <t>grid: Tile[][]</t>
-  </si>
-  <si>
-    <t>posX: int</t>
-  </si>
-  <si>
-    <t>posY: int</t>
-  </si>
-  <si>
-    <t>getPosX(): int</t>
-  </si>
-  <si>
-    <t>getPosY(): int</t>
-  </si>
-  <si>
-    <t>wallNorth: Wall</t>
-  </si>
-  <si>
-    <t>wallEast: Wall</t>
-  </si>
-  <si>
-    <t>wallSouth: Wall</t>
-  </si>
-  <si>
-    <t>wallWest: Wall</t>
-  </si>
-  <si>
-    <t>getWalls(): Walls[4]</t>
   </si>
   <si>
     <t>Point</t>
@@ -254,12 +224,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -384,37 +354,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -429,10 +373,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1251,7 +1193,7 @@
   <dimension ref="A2:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,9 +1261,9 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="4"/>
@@ -1332,10 +1274,13 @@
         <v>19</v>
       </c>
       <c r="K7" s="4"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="6"/>
@@ -1344,8 +1289,9 @@
       <c r="H8" s="4"/>
       <c r="J8" s="3"/>
       <c r="K8" s="4"/>
-      <c r="O8" s="16"/>
-      <c r="Q8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
     </row>
     <row r="9" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1358,7 +1304,8 @@
       <c r="H9" s="4"/>
       <c r="J9" s="3"/>
       <c r="K9" s="4"/>
-      <c r="O9" s="17"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
       <c r="Q9" s="15"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
@@ -1377,7 +1324,7 @@
     </row>
     <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="4"/>
@@ -1423,7 +1370,7 @@
     </row>
     <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="6"/>
@@ -1448,11 +1395,9 @@
       </c>
       <c r="P18" s="12"/>
       <c r="Q18" s="8"/>
-      <c r="S18" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="T18" s="12"/>
-      <c r="U18" s="8"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1474,15 +1419,13 @@
       <c r="L19" s="10"/>
       <c r="M19" s="4"/>
       <c r="O19" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="P19" s="9"/>
       <c r="Q19" s="2"/>
-      <c r="S19" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="S19" s="10"/>
       <c r="T19" s="10"/>
-      <c r="U19" s="4"/>
+      <c r="U19" s="10"/>
     </row>
     <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
@@ -1502,15 +1445,13 @@
       <c r="L20" s="10"/>
       <c r="M20" s="4"/>
       <c r="O20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="4"/>
-      <c r="S20" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="S20" s="10"/>
       <c r="T20" s="10"/>
-      <c r="U20" s="4"/>
+      <c r="U20" s="10"/>
     </row>
     <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
@@ -1530,11 +1471,9 @@
       <c r="O21" s="5"/>
       <c r="P21" s="11"/>
       <c r="Q21" s="6"/>
-      <c r="S21" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="S21" s="10"/>
       <c r="T21" s="10"/>
-      <c r="U21" s="4"/>
+      <c r="U21" s="10"/>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="5" t="s">
@@ -1552,11 +1491,9 @@
       <c r="O22" s="1"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="2"/>
-      <c r="S22" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="S22" s="10"/>
       <c r="T22" s="10"/>
-      <c r="U22" s="4"/>
+      <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="1" t="s">
@@ -1576,11 +1513,9 @@
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="4"/>
-      <c r="S23" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="S23" s="10"/>
       <c r="T23" s="10"/>
-      <c r="U23" s="4"/>
+      <c r="U23" s="10"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
@@ -1600,11 +1535,9 @@
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="4"/>
-      <c r="S24" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="S24" s="10"/>
       <c r="T24" s="10"/>
-      <c r="U24" s="4"/>
+      <c r="U24" s="10"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D25" s="13" t="s">
@@ -1624,9 +1557,9 @@
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="4"/>
-      <c r="S25" s="3"/>
+      <c r="S25" s="10"/>
       <c r="T25" s="10"/>
-      <c r="U25" s="4"/>
+      <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
@@ -1642,9 +1575,9 @@
       <c r="O26" s="3"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="4"/>
-      <c r="S26" s="3"/>
+      <c r="S26" s="10"/>
       <c r="T26" s="10"/>
-      <c r="U26" s="4"/>
+      <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="5"/>
@@ -1660,9 +1593,9 @@
       <c r="O27" s="5"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="6"/>
-      <c r="S27" s="3"/>
+      <c r="S27" s="10"/>
       <c r="T27" s="10"/>
-      <c r="U27" s="4"/>
+      <c r="U27" s="10"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G28" s="3" t="s">
@@ -1670,99 +1603,93 @@
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="4"/>
-      <c r="S28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="T28" s="9"/>
-      <c r="U28" s="2"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G29" s="3"/>
       <c r="H29" s="10"/>
       <c r="I29" s="4"/>
-      <c r="S29" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="S29" s="10"/>
       <c r="T29" s="10"/>
-      <c r="U29" s="4"/>
+      <c r="U29" s="10"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G30" s="3"/>
       <c r="H30" s="10"/>
       <c r="I30" s="4"/>
-      <c r="S30" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="S30" s="10"/>
       <c r="T30" s="10"/>
-      <c r="U30" s="4"/>
+      <c r="U30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G31" s="3"/>
       <c r="H31" s="10"/>
       <c r="I31" s="4"/>
       <c r="O31" s="7" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="P31" s="8"/>
-      <c r="S31" s="3"/>
+      <c r="S31" s="10"/>
       <c r="T31" s="10"/>
-      <c r="U31" s="4"/>
+      <c r="U31" s="10"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G32" s="3"/>
       <c r="H32" s="10"/>
       <c r="I32" s="4"/>
       <c r="O32" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="P32" s="4"/>
-      <c r="S32" s="3"/>
+      <c r="S32" s="10"/>
       <c r="T32" s="10"/>
-      <c r="U32" s="4"/>
+      <c r="U32" s="10"/>
     </row>
     <row r="33" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G33" s="5"/>
       <c r="H33" s="11"/>
       <c r="I33" s="6"/>
       <c r="O33" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="P33" s="4"/>
-      <c r="S33" s="3"/>
+      <c r="S33" s="10"/>
       <c r="T33" s="10"/>
-      <c r="U33" s="4"/>
+      <c r="U33" s="10"/>
     </row>
     <row r="34" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O34" s="5"/>
       <c r="P34" s="6"/>
-      <c r="S34" s="3"/>
+      <c r="S34" s="10"/>
       <c r="T34" s="10"/>
-      <c r="U34" s="4"/>
-    </row>
-    <row r="35" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U34" s="10"/>
+    </row>
+    <row r="35" spans="7:21" x14ac:dyDescent="0.25">
       <c r="O35" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="P35" s="4"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="6"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
     </row>
     <row r="36" spans="7:21" x14ac:dyDescent="0.25">
       <c r="O36" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="P36" s="4"/>
     </row>
     <row r="37" spans="7:21" x14ac:dyDescent="0.25">
       <c r="O37" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="P37" s="4"/>
     </row>
     <row r="38" spans="7:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O38" s="5" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="P38" s="6"/>
     </row>

</xml_diff>